<commit_message>
update cookie sync model with real-world data
</commit_message>
<xml_diff>
--- a/docs/pc_emissions_model.xlsx
+++ b/docs/pc_emissions_model.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFD80F2-8FD4-424D-B8BD-9C1E3334C4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCCE6C4-9429-8045-9DAD-7CC461A79C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
+    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="1" r:id="rId1"/>
     <sheet name="TV" sheetId="2" r:id="rId2"/>
+    <sheet name="Cookies" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Desktop</t>
   </si>
@@ -100,18 +101,49 @@
   </si>
   <si>
     <t>TV System</t>
+  </si>
+  <si>
+    <t>Emissions from cookies - representative</t>
+  </si>
+  <si>
+    <t>Page views per month</t>
+  </si>
+  <si>
+    <t>Ad tech partners (direct and indirect)</t>
+  </si>
+  <si>
+    <t>Cookie syncs per page view</t>
+  </si>
+  <si>
+    <t>Cookie syncs per month</t>
+  </si>
+  <si>
+    <t>Data transfer from cookie syncs (GB)</t>
+  </si>
+  <si>
+    <t>Electricity use from data transfer (kWh)</t>
+  </si>
+  <si>
+    <t>Emissions from data transfer - US (gCO2e)</t>
+  </si>
+  <si>
+    <t>Server-side emissions (gCO2e)</t>
+  </si>
+  <si>
+    <t>Total emissions (mt CO2e)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,6 +152,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -135,12 +175,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -149,12 +198,20 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -613,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F090A55B-62F6-0F42-8666-160B97953F95}">
   <dimension ref="E10:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -735,4 +792,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF20CB-EC62-8543-9C04-FE3F502E9283}">
+  <dimension ref="D7:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="7">
+        <f>0.2*E9</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="8">
+        <f>E10*E8</f>
+        <v>50000000000</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="9">
+        <f>1.3*E11/1024/1024</f>
+        <v>61988.83056640625</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="9">
+        <f>E13*0.03</f>
+        <v>1859.6649169921875</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="9">
+        <f>347*E14</f>
+        <v>645303.72619628906</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="9">
+        <f>0.000365*E11</f>
+        <v>18250000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="10">
+        <f>(E17+E15)/1000000</f>
+        <v>18.895303726196289</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
use yahoo.com for the example
</commit_message>
<xml_diff>
--- a/docs/pc_emissions_model.xlsx
+++ b/docs/pc_emissions_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bokelley/src/methodology/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCCE6C4-9429-8045-9DAD-7CC461A79C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFA9FAC-620E-274B-BF9D-A4D634762187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{35CF7F97-C8CD-114B-B6E3-1E1EA0AAA903}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Desktop</t>
   </si>
@@ -103,12 +103,6 @@
     <t>TV System</t>
   </si>
   <si>
-    <t>Emissions from cookies - representative</t>
-  </si>
-  <si>
-    <t>Page views per month</t>
-  </si>
-  <si>
     <t>Ad tech partners (direct and indirect)</t>
   </si>
   <si>
@@ -130,18 +124,28 @@
     <t>Server-side emissions (gCO2e)</t>
   </si>
   <si>
-    <t>Total emissions (mt CO2e)</t>
+    <t>Emissions from cookies - yahoo.com</t>
+  </si>
+  <si>
+    <t>Page views per month (B)</t>
+  </si>
+  <si>
+    <t>Source: SimilarWeb</t>
+  </si>
+  <si>
+    <t>Total annual emissions (mt CO2e)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -204,14 +208,14 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -796,10 +800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBF20CB-EC62-8543-9C04-FE3F502E9283}">
-  <dimension ref="D7:E19"/>
+  <dimension ref="D7:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,89 +812,92 @@
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D7" s="5" t="s">
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="10">
+        <v>18.942</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>23</v>
       </c>
       <c r="E9">
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="7">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="5">
         <f>0.2*E9</f>
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="6">
+        <f>E10*E8</f>
+        <v>947.1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="7">
+        <f>1.3*E11*1000000000/1024/1024</f>
+        <v>1174192.4285888672</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="8">
-        <f>E10*E8</f>
-        <v>50000000000</v>
-      </c>
-    </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
+      <c r="E14" s="7">
+        <f>E13*0.03</f>
+        <v>35225.772857666016</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="9">
-        <f>1.3*E11/1024/1024</f>
-        <v>61988.83056640625</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="9">
-        <f>E13*0.03</f>
-        <v>1859.6649169921875</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <f>347*E14</f>
-        <v>645303.72619628906</v>
+        <v>12223343.181610107</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="9">
-        <f>0.000365*E11</f>
-        <v>18250000</v>
+        <v>27</v>
+      </c>
+      <c r="E17" s="7">
+        <f>0.000365*E11*1000000000</f>
+        <v>345691500</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="10">
-        <f>(E17+E15)/1000000</f>
-        <v>18.895303726196289</v>
+        <v>31</v>
+      </c>
+      <c r="E19" s="8">
+        <f>(E17+E15)/1000000*12</f>
+        <v>4294.9781181793205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>